<commit_message>
backup Sun Jun 14 17:21:23 PDT 2020
</commit_message>
<xml_diff>
--- a/data/raw/2020-06-12/sheet_all_tabs.xlsx
+++ b/data/raw/2020-06-12/sheet_all_tabs.xlsx
@@ -1302,14 +1302,17 @@
           <t>Sweden</t>
         </is>
       </c>
+      <c r="E2">
+        <v>8534.200000000001</v>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1339,14 +1342,17 @@
           <t>United Kingdom</t>
         </is>
       </c>
+      <c r="E3">
+        <v>43962.01</v>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -1376,14 +1382,17 @@
           <t>Italy</t>
         </is>
       </c>
+      <c r="E4">
+        <v>35229.87</v>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -1413,14 +1422,17 @@
           <t>Spain</t>
         </is>
       </c>
+      <c r="E5">
+        <v>27006.12</v>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -1450,14 +1462,17 @@
           <t>Belgium</t>
         </is>
       </c>
+      <c r="E6">
+        <v>11093.42</v>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1487,14 +1502,17 @@
           <t>France</t>
         </is>
       </c>
+      <c r="E7">
+        <v>34602.38</v>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1524,14 +1542,17 @@
           <t>Germany</t>
         </is>
       </c>
+      <c r="E8">
+        <v>9500.376</v>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1561,14 +1582,17 @@
           <t>Netherlands</t>
         </is>
       </c>
+      <c r="E9">
+        <v>6598.558</v>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1598,14 +1622,17 @@
           <t>Switzerland</t>
         </is>
       </c>
+      <c r="E10">
+        <v>3398.807</v>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>04</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1633,16 +1660,6 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>Canada</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>24</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">

</xml_diff>